<commit_message>
Add 'weight_type' to the Score model and update the Scoring file format
</commit_message>
<xml_diff>
--- a/curation/templates/ScoringFileSchema.xlsx
+++ b/curation/templates/ScoringFileSchema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_curation/curation/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_weight_type/curation/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E471E1E6-97B8-D44B-A3C3-19FFD107B0F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F1236-1811-2A4C-B427-905F625036E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37040" yWindow="2540" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EEB73C32-DC8F-1B4B-BFFE-27FF268BF4B0}"/>
+    <workbookView xWindow="40180" yWindow="4960" windowWidth="28800" windowHeight="16260" xr2:uid="{EEB73C32-DC8F-1B4B-BFFE-27FF268BF4B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Column Header</t>
   </si>
@@ -89,15 +89,6 @@
   </si>
   <si>
     <t>Value of the effect that is multiplied with the dosage.</t>
-  </si>
-  <si>
-    <t>weight_type</t>
-  </si>
-  <si>
-    <t>Type of Weight</t>
-  </si>
-  <si>
-    <t>Whether the author supplied Variant Weight is a: beta (effect size), or something like an OR/HR (odds/hazard ratio)</t>
   </si>
   <si>
     <t>allelefrequency_effect</t>
@@ -314,8 +305,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,26 +623,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BC9083-E881-AF4A-862C-089B33A08BC9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="8">
-        <v>44337</v>
+        <v>44459</v>
       </c>
     </row>
   </sheetData>
@@ -661,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040732F3-A12D-E644-952D-3CC6007072F3}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,10 +733,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>17</v>
@@ -781,59 +772,59 @@
         <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>59</v>
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -870,35 +861,24 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>